<commit_message>
corregi bug de enter en ventas
</commit_message>
<xml_diff>
--- a/cajas-diarias/caja-2023-09-12.xlsx
+++ b/cajas-diarias/caja-2023-09-12.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -448,9 +448,55 @@
         <v>EFECTIVO</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>-</v>
+      </c>
+      <c r="B3" t="str">
+        <v>100</v>
+      </c>
+      <c r="C3" t="str">
+        <v>SUELTO</v>
+      </c>
+      <c r="D3" t="str">
+        <v>-</v>
+      </c>
+      <c r="E3" t="str">
+        <v>-</v>
+      </c>
+      <c r="F3" t="str">
+        <v>0</v>
+      </c>
+      <c r="G3" t="str">
+        <v>EFECTIVO</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>-</v>
+      </c>
+      <c r="B4" t="str">
+        <v>20000</v>
+      </c>
+      <c r="C4" t="str">
+        <v>SUELTO</v>
+      </c>
+      <c r="D4" t="str">
+        <v>-</v>
+      </c>
+      <c r="E4" t="str">
+        <v>-</v>
+      </c>
+      <c r="F4" t="str">
+        <v>0</v>
+      </c>
+      <c r="G4" t="str">
+        <v>DEBITO</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>